<commit_message>
adicionando planilhas para visualizacao do PRIM
</commit_message>
<xml_diff>
--- a/boruta_results.xlsx
+++ b/boruta_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\2019.1-3dp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DB5719-5685-4678-856A-282911B6CB43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1434DE5-85D2-4F6B-B07C-5AF60BD1E34E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,7 +651,7 @@
   <dimension ref="A1:M631"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>